<commit_message>
how to clean data
</commit_message>
<xml_diff>
--- a/starbucks_bakery.xlsx
+++ b/starbucks_bakery.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chula-my.sharepoint.com/personal/prasert_k_chula_ac_th/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prasert\1drv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97F8879B-42FA-44B7-8E73-5686C0F7000F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161DD5F6-3B16-47B5-9594-A7F8E9692553}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{308F07E6-74DA-4B61-B628-237ADA91CCA0}"/>
   </bookViews>
@@ -736,7 +736,7 @@
     </r>
   </si>
   <si>
-    <t>Item</t>
+    <t>Product Name</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>